<commit_message>
Added multi-file auto framework
</commit_message>
<xml_diff>
--- a/Auto File Details.xlsx
+++ b/Auto File Details.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
   <si>
     <t>BLUE LEFT</t>
   </si>
@@ -69,6 +69,42 @@
   </si>
   <si>
     <t>B4</t>
+  </si>
+  <si>
+    <t>First.csv</t>
+  </si>
+  <si>
+    <t>FILES</t>
+  </si>
+  <si>
+    <t>INFO</t>
+  </si>
+  <si>
+    <t>Drive behind Switch</t>
+  </si>
+  <si>
+    <t>Switch_Close.csv</t>
+  </si>
+  <si>
+    <t>Switch_Far.csv</t>
+  </si>
+  <si>
+    <t>Scale_Close.csv</t>
+  </si>
+  <si>
+    <t>Scale_Far.csv</t>
+  </si>
+  <si>
+    <t>Score in scale platform directly behind robot</t>
+  </si>
+  <si>
+    <t>Score in scale platform across from robot</t>
+  </si>
+  <si>
+    <t>Score in far switch platform &amp; collect block</t>
+  </si>
+  <si>
+    <t>Score in close switch platform &amp; collect block</t>
   </si>
 </sst>
 </file>
@@ -429,10 +465,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{577C4244-3D9A-4626-9C52-70F76AB2C2FA}">
-  <dimension ref="A1:F5"/>
+  <dimension ref="A1:F14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -501,6 +537,54 @@
         <v>14</v>
       </c>
     </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A9" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>15</v>
+      </c>
+      <c r="B10" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>19</v>
+      </c>
+      <c r="B11" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>20</v>
+      </c>
+      <c r="B12" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>21</v>
+      </c>
+      <c r="B13" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>22</v>
+      </c>
+      <c r="B14" t="s">
+        <v>24</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>